<commit_message>
Adding exception handling and property types
</commit_message>
<xml_diff>
--- a/files/students.xlsx
+++ b/files/students.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>STUDENTS LIST</t>
   </si>
@@ -28,22 +28,31 @@
     <t>Ipsum</t>
   </si>
   <si>
-    <t>Dolor</t>
-  </si>
-  <si>
-    <t>Far</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>aaaa</t>
-  </si>
-  <si>
     <t>Birthdate</t>
   </si>
   <si>
     <t>18/07/2017</t>
+  </si>
+  <si>
+    <t>Join date</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>IS GOOD</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Haha</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -79,9 +88,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,68 +397,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C23"/>
+  <dimension ref="A2:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>45857</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1">
         <v>43308</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <v>42935</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
       <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1">
+        <v>42935</v>
+      </c>
+      <c r="D7" s="1">
+        <v>42935</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>